<commit_message>
Updated functions to get activity periods
</commit_message>
<xml_diff>
--- a/data/Schedule.xlsx
+++ b/data/Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Biking</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Tetherball</t>
-  </si>
-  <si>
-    <t>Uberball</t>
   </si>
   <si>
     <t>Camp Songs</t>
@@ -432,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,95 +461,210 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
+      <c r="F4">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
-        <v>31</v>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>